<commit_message>
changed model architecture to resnet
</commit_message>
<xml_diff>
--- a/models-pain.xlsx
+++ b/models-pain.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leeds365-my.sharepoint.com/personal/sc20dzi_leeds_ac_uk/Documents/Year 3/Semester 2/Individual Project/pain-detection-cats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="6_{5BED099B-C9F0-B74F-8F8D-086DFAE8EDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9E695E7-C5BF-3A48-96DC-D4E827D2EBE6}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="6_{5BED099B-C9F0-B74F-8F8D-086DFAE8EDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A605C374-4DCE-1A40-AAE7-AF1F7E721B56}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27160" windowHeight="10720" xr2:uid="{1B0D5C52-EC28-504B-82BB-4D697B131FA2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>id</t>
   </si>
@@ -59,9 +59,6 @@
     <t>batch size</t>
   </si>
   <si>
-    <t>3 + 1</t>
-  </si>
-  <si>
     <t>layers (conv + dense)</t>
   </si>
   <si>
@@ -74,14 +71,38 @@
     <t>leaky relu</t>
   </si>
   <si>
-    <t>4 + 1</t>
+    <t>4 + 2</t>
+  </si>
+  <si>
+    <t>5 + 2</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>loss - mae</t>
+  </si>
+  <si>
+    <t>6 + 2</t>
+  </si>
+  <si>
+    <t>3 + 2</t>
+  </si>
+  <si>
+    <t>resnet</t>
+  </si>
+  <si>
+    <t>loss</t>
+  </si>
+  <si>
+    <t>f1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -110,6 +131,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -132,11 +159,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -153,6 +183,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -452,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716DD8F1-517E-834D-909E-B26119B5ADB6}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,9 +503,10 @@
     <col min="8" max="8" width="12.6640625" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11.6640625" customWidth="1"/>
+    <col min="14" max="15" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,10 +517,10 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -499,11 +534,32 @@
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="1"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -514,26 +570,33 @@
         <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3">
         <v>0.52171242237090998</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="3">
         <v>0.64098799228668202</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="3">
         <v>0.72229659557342496</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="3">
         <v>-6.4525775611400604E-2</v>
       </c>
-      <c r="J2" s="2"/>
+      <c r="J2" s="3"/>
       <c r="K2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" s="6">
+        <v>10</v>
+      </c>
+      <c r="O2" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -544,27 +607,29 @@
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.71232515573501498</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0.62415611743927002</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0.84399360418319702</v>
-      </c>
-      <c r="I3" s="2">
-        <v>-0.45740634202957098</v>
-      </c>
-      <c r="J3" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.52482253313064497</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.64298886060714699</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.72444635629653897</v>
+      </c>
+      <c r="I3" s="3">
+        <v>-7.0619694888591697E-2</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.34369701147079401</v>
+      </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -575,64 +640,171 @@
         <v>32</v>
       </c>
       <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.53243720531463601</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.64317995309829701</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.72968298196792603</v>
+      </c>
+      <c r="I4" s="3">
+        <v>-8.2468770444393102E-2</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.54431802034377996</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.6491060256958</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.737779140472412</v>
+      </c>
+      <c r="I5" s="3">
+        <v>-0.11175499856472</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="2">
-        <v>0.53243720531463601</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0.64317995309829701</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0.72968298196792603</v>
-      </c>
-      <c r="I4" s="2">
-        <v>-8.2468770444393102E-2</v>
-      </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="F6" s="3">
+        <v>0.51209849119186401</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.64289569854736295</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.71561062335967995</v>
+      </c>
+      <c r="I6" s="4">
+        <v>-4.95873801410198E-2</v>
+      </c>
+      <c r="J6" s="3"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>64</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.53058451414108199</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.63775438070297197</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.72841233015060403</v>
+      </c>
+      <c r="I7" s="3">
+        <v>-7.8715518116950906E-2</v>
+      </c>
+      <c r="J7" s="3"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="2"/>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.618990898132324</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.84221649169921797</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.91772353649139404</v>
+      </c>
+      <c r="I8" s="3">
+        <v>-0.72106808423995905</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.51667612791061401</v>
+      </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>64</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.50900489091873102</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.64179110527038497</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.71344578266143799</v>
+      </c>
+      <c r="I9" s="2">
+        <v>-4.2272929102182298E-2</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.34313172101974398</v>
+      </c>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -640,7 +812,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -648,15 +820,15 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="H12" s="3"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -664,7 +836,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -672,7 +844,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -680,7 +852,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>

</xml_diff>